<commit_message>
Revise figures, supp figures, and supp tables for overleaf
</commit_message>
<xml_diff>
--- a/results/outputs/main/v4/supplemental_tables/marker_gene_matrix_table.xlsx
+++ b/results/outputs/main/v4/supplemental_tables/marker_gene_matrix_table.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="126">
+  <si>
+    <t>Gene</t>
+  </si>
   <si>
     <t>hESC</t>
   </si>
@@ -40,6 +43,258 @@
     <t>D2LtM</t>
   </si>
   <si>
+    <t>ENSG00000008311</t>
+  </si>
+  <si>
+    <t>ENSG00000018625</t>
+  </si>
+  <si>
+    <t>ENSG00000019549</t>
+  </si>
+  <si>
+    <t>ENSG00000026025</t>
+  </si>
+  <si>
+    <t>ENSG00000039068</t>
+  </si>
+  <si>
+    <t>ENSG00000042493</t>
+  </si>
+  <si>
+    <t>ENSG00000053438</t>
+  </si>
+  <si>
+    <t>ENSG00000075340</t>
+  </si>
+  <si>
+    <t>ENSG00000079102</t>
+  </si>
+  <si>
+    <t>ENSG00000092068</t>
+  </si>
+  <si>
+    <t>ENSG00000101850</t>
+  </si>
+  <si>
+    <t>ENSG00000104267</t>
+  </si>
+  <si>
+    <t>ENSG00000107438</t>
+  </si>
+  <si>
+    <t>ENSG00000107984</t>
+  </si>
+  <si>
+    <t>ENSG00000111057</t>
+  </si>
+  <si>
+    <t>ENSG00000111816</t>
+  </si>
+  <si>
+    <t>ENSG00000114251</t>
+  </si>
+  <si>
+    <t>ENSG00000116729</t>
+  </si>
+  <si>
+    <t>ENSG00000118640</t>
+  </si>
+  <si>
+    <t>ENSG00000120738</t>
+  </si>
+  <si>
+    <t>ENSG00000127863</t>
+  </si>
+  <si>
+    <t>ENSG00000130203</t>
+  </si>
+  <si>
+    <t>ENSG00000132297</t>
+  </si>
+  <si>
+    <t>ENSG00000132669</t>
+  </si>
+  <si>
+    <t>ENSG00000133636</t>
+  </si>
+  <si>
+    <t>ENSG00000134363</t>
+  </si>
+  <si>
+    <t>ENSG00000134817</t>
+  </si>
+  <si>
+    <t>ENSG00000134853</t>
+  </si>
+  <si>
+    <t>ENSG00000136167</t>
+  </si>
+  <si>
+    <t>ENSG00000137831</t>
+  </si>
+  <si>
+    <t>ENSG00000137868</t>
+  </si>
+  <si>
+    <t>ENSG00000138061</t>
+  </si>
+  <si>
+    <t>ENSG00000138795</t>
+  </si>
+  <si>
+    <t>ENSG00000138821</t>
+  </si>
+  <si>
+    <t>ENSG00000139318</t>
+  </si>
+  <si>
+    <t>ENSG00000140937</t>
+  </si>
+  <si>
+    <t>ENSG00000141449</t>
+  </si>
+  <si>
+    <t>ENSG00000143320</t>
+  </si>
+  <si>
+    <t>ENSG00000145147</t>
+  </si>
+  <si>
+    <t>ENSG00000147010</t>
+  </si>
+  <si>
+    <t>ENSG00000147601</t>
+  </si>
+  <si>
+    <t>ENSG00000151150</t>
+  </si>
+  <si>
+    <t>ENSG00000153363</t>
+  </si>
+  <si>
+    <t>ENSG00000153721</t>
+  </si>
+  <si>
+    <t>ENSG00000156966</t>
+  </si>
+  <si>
+    <t>ENSG00000158270</t>
+  </si>
+  <si>
+    <t>ENSG00000158710</t>
+  </si>
+  <si>
+    <t>ENSG00000161249</t>
+  </si>
+  <si>
+    <t>ENSG00000162433</t>
+  </si>
+  <si>
+    <t>ENSG00000162551</t>
+  </si>
+  <si>
+    <t>ENSG00000163132</t>
+  </si>
+  <si>
+    <t>ENSG00000163492</t>
+  </si>
+  <si>
+    <t>ENSG00000164741</t>
+  </si>
+  <si>
+    <t>ENSG00000166450</t>
+  </si>
+  <si>
+    <t>ENSG00000166900</t>
+  </si>
+  <si>
+    <t>ENSG00000169122</t>
+  </si>
+  <si>
+    <t>ENSG00000169554</t>
+  </si>
+  <si>
+    <t>ENSG00000169764</t>
+  </si>
+  <si>
+    <t>ENSG00000170421</t>
+  </si>
+  <si>
+    <t>ENSG00000170542</t>
+  </si>
+  <si>
+    <t>ENSG00000170961</t>
+  </si>
+  <si>
+    <t>ENSG00000171345</t>
+  </si>
+  <si>
+    <t>ENSG00000174469</t>
+  </si>
+  <si>
+    <t>ENSG00000179059</t>
+  </si>
+  <si>
+    <t>ENSG00000181744</t>
+  </si>
+  <si>
+    <t>ENSG00000182718</t>
+  </si>
+  <si>
+    <t>ENSG00000185155</t>
+  </si>
+  <si>
+    <t>ENSG00000185920</t>
+  </si>
+  <si>
+    <t>ENSG00000197461</t>
+  </si>
+  <si>
+    <t>ENSG00000197747</t>
+  </si>
+  <si>
+    <t>ENSG00000215866</t>
+  </si>
+  <si>
+    <t>ENSG00000234787</t>
+  </si>
+  <si>
+    <t>ENSG00000236673</t>
+  </si>
+  <si>
+    <t>ENSG00000237515</t>
+  </si>
+  <si>
+    <t>ENSG00000240563</t>
+  </si>
+  <si>
+    <t>ENSG00000241186</t>
+  </si>
+  <si>
+    <t>ENSG00000243004</t>
+  </si>
+  <si>
+    <t>ENSG00000249532</t>
+  </si>
+  <si>
+    <t>ENSG00000250305</t>
+  </si>
+  <si>
+    <t>ENSG00000254277</t>
+  </si>
+  <si>
+    <t>ENSG00000254339</t>
+  </si>
+  <si>
+    <t>ENSG00000260342</t>
+  </si>
+  <si>
+    <t>ENSG00000260834</t>
+  </si>
+  <si>
+    <t>ENSG00000280623</t>
+  </si>
+  <si>
     <t>B cells</t>
   </si>
   <si>
@@ -55,10 +310,88 @@
     <t>other</t>
   </si>
   <si>
+    <t>CCL5</t>
+  </si>
+  <si>
+    <t>CD19</t>
+  </si>
+  <si>
+    <t>CD2</t>
+  </si>
+  <si>
+    <t>CD3D</t>
+  </si>
+  <si>
+    <t>CD3E</t>
+  </si>
+  <si>
+    <t>CD3G</t>
+  </si>
+  <si>
+    <t>CD4</t>
+  </si>
+  <si>
+    <t>CD74</t>
+  </si>
+  <si>
+    <t>CD79A</t>
+  </si>
+  <si>
+    <t>CD79B</t>
+  </si>
+  <si>
+    <t>CD8A</t>
+  </si>
+  <si>
+    <t>CD8B</t>
+  </si>
+  <si>
+    <t>CXCR5</t>
+  </si>
+  <si>
+    <t>EOMES</t>
+  </si>
+  <si>
+    <t>GZMA</t>
+  </si>
+  <si>
+    <t>ICA1</t>
+  </si>
+  <si>
+    <t>ICOS</t>
+  </si>
+  <si>
+    <t>IL7R</t>
+  </si>
+  <si>
+    <t>MS4A1</t>
+  </si>
+  <si>
+    <t>NKG7</t>
+  </si>
+  <si>
+    <t>PDCD1</t>
+  </si>
+  <si>
+    <t>ST8SIA1</t>
+  </si>
+  <si>
+    <t>TNFRSF4</t>
+  </si>
+  <si>
+    <t>TRAC</t>
+  </si>
+  <si>
     <t>IGKC</t>
   </si>
   <si>
     <t>IGLC</t>
+  </si>
+  <si>
+    <t>IGLC2</t>
+  </si>
+  <si>
+    <t>IGLC3</t>
   </si>
 </sst>
 </file>
@@ -134,13 +467,16 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1.0</v>
+      <c r="A2" t="s">
+        <v>9</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C2" t="n">
         <v>0.0</v>
@@ -160,19 +496,22 @@
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
+      <c r="I2" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1.0</v>
+      <c r="A3" t="s">
+        <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
       </c>
       <c r="D3" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E3" t="n">
         <v>1.0</v>
@@ -186,13 +525,16 @@
       <c r="H3" t="n">
         <v>1.0</v>
       </c>
+      <c r="I3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>0.0</v>
+      <c r="A4" t="s">
+        <v>11</v>
       </c>
       <c r="B4" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
@@ -212,10 +554,13 @@
       <c r="H4" t="n">
         <v>1.0</v>
       </c>
+      <c r="I4" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>0.0</v>
+      <c r="A5" t="s">
+        <v>12</v>
       </c>
       <c r="B5" t="n">
         <v>0.0</v>
@@ -224,7 +569,7 @@
         <v>0.0</v>
       </c>
       <c r="D5" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E5" t="n">
         <v>1.0</v>
@@ -238,10 +583,13 @@
       <c r="H5" t="n">
         <v>1.0</v>
       </c>
+      <c r="I5" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1.0</v>
+      <c r="A6" t="s">
+        <v>13</v>
       </c>
       <c r="B6" t="n">
         <v>1.0</v>
@@ -256,18 +604,21 @@
         <v>1.0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
       </c>
       <c r="H6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I6" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>1.0</v>
+      <c r="A7" t="s">
+        <v>14</v>
       </c>
       <c r="B7" t="n">
         <v>1.0</v>
@@ -282,18 +633,21 @@
         <v>1.0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G7" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H7" t="n">
         <v>1.0</v>
       </c>
+      <c r="I7" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>0.0</v>
+      <c r="A8" t="s">
+        <v>15</v>
       </c>
       <c r="B8" t="n">
         <v>0.0</v>
@@ -305,10 +659,10 @@
         <v>0.0</v>
       </c>
       <c r="E8" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G8" t="n">
         <v>0.0</v>
@@ -316,10 +670,13 @@
       <c r="H8" t="n">
         <v>0.0</v>
       </c>
+      <c r="I8" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>1.0</v>
+      <c r="A9" t="s">
+        <v>16</v>
       </c>
       <c r="B9" t="n">
         <v>1.0</v>
@@ -334,18 +691,21 @@
         <v>1.0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H9" t="n">
         <v>1.0</v>
       </c>
+      <c r="I9" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>1.0</v>
+      <c r="A10" t="s">
+        <v>17</v>
       </c>
       <c r="B10" t="n">
         <v>1.0</v>
@@ -354,10 +714,10 @@
         <v>1.0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F10" t="n">
         <v>1.0</v>
@@ -368,10 +728,13 @@
       <c r="H10" t="n">
         <v>1.0</v>
       </c>
+      <c r="I10" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>1.0</v>
+      <c r="A11" t="s">
+        <v>18</v>
       </c>
       <c r="B11" t="n">
         <v>1.0</v>
@@ -386,18 +749,21 @@
         <v>1.0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G11" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H11" t="n">
         <v>1.0</v>
       </c>
+      <c r="I11" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>1.0</v>
+      <c r="A12" t="s">
+        <v>19</v>
       </c>
       <c r="B12" t="n">
         <v>1.0</v>
@@ -412,18 +778,21 @@
         <v>1.0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G12" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H12" t="n">
         <v>1.0</v>
       </c>
+      <c r="I12" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>1.0</v>
+      <c r="A13" t="s">
+        <v>20</v>
       </c>
       <c r="B13" t="n">
         <v>1.0</v>
@@ -438,18 +807,21 @@
         <v>1.0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G13" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H13" t="n">
         <v>1.0</v>
       </c>
+      <c r="I13" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>1.0</v>
+      <c r="A14" t="s">
+        <v>21</v>
       </c>
       <c r="B14" t="n">
         <v>1.0</v>
@@ -464,21 +836,24 @@
         <v>1.0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G14" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H14" t="n">
         <v>1.0</v>
       </c>
+      <c r="I14" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>0.0</v>
+      <c r="A15" t="s">
+        <v>22</v>
       </c>
       <c r="B15" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C15" t="n">
         <v>1.0</v>
@@ -487,21 +862,24 @@
         <v>1.0</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F15" t="n">
         <v>0.0</v>
       </c>
       <c r="G15" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I15" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>1.0</v>
+      <c r="A16" t="s">
+        <v>23</v>
       </c>
       <c r="B16" t="n">
         <v>1.0</v>
@@ -516,18 +894,21 @@
         <v>1.0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G16" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H16" t="n">
         <v>1.0</v>
       </c>
+      <c r="I16" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>1.0</v>
+      <c r="A17" t="s">
+        <v>24</v>
       </c>
       <c r="B17" t="n">
         <v>1.0</v>
@@ -536,10 +917,10 @@
         <v>1.0</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E17" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F17" t="n">
         <v>1.0</v>
@@ -550,13 +931,16 @@
       <c r="H17" t="n">
         <v>1.0</v>
       </c>
+      <c r="I17" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>0.0</v>
+      <c r="A18" t="s">
+        <v>25</v>
       </c>
       <c r="B18" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C18" t="n">
         <v>1.0</v>
@@ -576,13 +960,16 @@
       <c r="H18" t="n">
         <v>1.0</v>
       </c>
+      <c r="I18" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>0.0</v>
+      <c r="A19" t="s">
+        <v>26</v>
       </c>
       <c r="B19" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C19" t="n">
         <v>1.0</v>
@@ -602,10 +989,13 @@
       <c r="H19" t="n">
         <v>1.0</v>
       </c>
+      <c r="I19" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>1.0</v>
+      <c r="A20" t="s">
+        <v>27</v>
       </c>
       <c r="B20" t="n">
         <v>1.0</v>
@@ -620,18 +1010,21 @@
         <v>1.0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G20" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H20" t="n">
         <v>1.0</v>
       </c>
+      <c r="I20" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>1.0</v>
+      <c r="A21" t="s">
+        <v>28</v>
       </c>
       <c r="B21" t="n">
         <v>1.0</v>
@@ -643,24 +1036,27 @@
         <v>1.0</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F21" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I21" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>0.0</v>
+      <c r="A22" t="s">
+        <v>29</v>
       </c>
       <c r="B22" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C22" t="n">
         <v>1.0</v>
@@ -678,12 +1074,15 @@
         <v>1.0</v>
       </c>
       <c r="H22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I22" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>1.0</v>
+      <c r="A23" t="s">
+        <v>30</v>
       </c>
       <c r="B23" t="n">
         <v>1.0</v>
@@ -698,24 +1097,27 @@
         <v>1.0</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G23" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H23" t="n">
         <v>1.0</v>
       </c>
+      <c r="I23" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>1.0</v>
+      <c r="A24" t="s">
+        <v>31</v>
       </c>
       <c r="B24" t="n">
         <v>1.0</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D24" t="n">
         <v>0.0</v>
@@ -732,10 +1134,13 @@
       <c r="H24" t="n">
         <v>0.0</v>
       </c>
+      <c r="I24" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>0.0</v>
+      <c r="A25" t="s">
+        <v>32</v>
       </c>
       <c r="B25" t="n">
         <v>0.0</v>
@@ -744,7 +1149,7 @@
         <v>0.0</v>
       </c>
       <c r="D25" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E25" t="n">
         <v>1.0</v>
@@ -758,13 +1163,16 @@
       <c r="H25" t="n">
         <v>1.0</v>
       </c>
+      <c r="I25" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>0.0</v>
+      <c r="A26" t="s">
+        <v>33</v>
       </c>
       <c r="B26" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C26" t="n">
         <v>1.0</v>
@@ -773,7 +1181,7 @@
         <v>1.0</v>
       </c>
       <c r="E26" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F26" t="n">
         <v>0.0</v>
@@ -782,15 +1190,18 @@
         <v>0.0</v>
       </c>
       <c r="H26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I26" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>0.0</v>
+      <c r="A27" t="s">
+        <v>34</v>
       </c>
       <c r="B27" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C27" t="n">
         <v>1.0</v>
@@ -808,15 +1219,18 @@
         <v>1.0</v>
       </c>
       <c r="H27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I27" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>0.0</v>
+      <c r="A28" t="s">
+        <v>35</v>
       </c>
       <c r="B28" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C28" t="n">
         <v>1.0</v>
@@ -836,13 +1250,16 @@
       <c r="H28" t="n">
         <v>1.0</v>
       </c>
+      <c r="I28" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>0.0</v>
+      <c r="A29" t="s">
+        <v>36</v>
       </c>
       <c r="B29" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C29" t="n">
         <v>1.0</v>
@@ -862,10 +1279,13 @@
       <c r="H29" t="n">
         <v>1.0</v>
       </c>
+      <c r="I29" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>1.0</v>
+      <c r="A30" t="s">
+        <v>37</v>
       </c>
       <c r="B30" t="n">
         <v>1.0</v>
@@ -877,7 +1297,7 @@
         <v>1.0</v>
       </c>
       <c r="E30" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F30" t="n">
         <v>0.0</v>
@@ -886,12 +1306,15 @@
         <v>0.0</v>
       </c>
       <c r="H30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I30" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>0.0</v>
+      <c r="A31" t="s">
+        <v>38</v>
       </c>
       <c r="B31" t="n">
         <v>0.0</v>
@@ -906,18 +1329,21 @@
         <v>0.0</v>
       </c>
       <c r="F31" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H31" t="n">
         <v>0.0</v>
       </c>
+      <c r="I31" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
-        <v>0.0</v>
+      <c r="A32" t="s">
+        <v>39</v>
       </c>
       <c r="B32" t="n">
         <v>0.0</v>
@@ -926,10 +1352,10 @@
         <v>0.0</v>
       </c>
       <c r="D32" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E32" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F32" t="n">
         <v>0.0</v>
@@ -940,10 +1366,13 @@
       <c r="H32" t="n">
         <v>0.0</v>
       </c>
+      <c r="I32" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
-        <v>0.0</v>
+      <c r="A33" t="s">
+        <v>40</v>
       </c>
       <c r="B33" t="n">
         <v>0.0</v>
@@ -955,7 +1384,7 @@
         <v>0.0</v>
       </c>
       <c r="E33" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F33" t="n">
         <v>1.0</v>
@@ -964,15 +1393,18 @@
         <v>1.0</v>
       </c>
       <c r="H33" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I33" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
-        <v>0.0</v>
+      <c r="A34" t="s">
+        <v>41</v>
       </c>
       <c r="B34" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C34" t="n">
         <v>1.0</v>
@@ -992,13 +1424,16 @@
       <c r="H34" t="n">
         <v>1.0</v>
       </c>
+      <c r="I34" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
-        <v>0.0</v>
+      <c r="A35" t="s">
+        <v>42</v>
       </c>
       <c r="B35" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C35" t="n">
         <v>1.0</v>
@@ -1007,7 +1442,7 @@
         <v>1.0</v>
       </c>
       <c r="E35" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F35" t="n">
         <v>0.0</v>
@@ -1018,10 +1453,13 @@
       <c r="H35" t="n">
         <v>0.0</v>
       </c>
+      <c r="I35" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
-        <v>1.0</v>
+      <c r="A36" t="s">
+        <v>43</v>
       </c>
       <c r="B36" t="n">
         <v>1.0</v>
@@ -1033,10 +1471,10 @@
         <v>1.0</v>
       </c>
       <c r="E36" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F36" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G36" t="n">
         <v>1.0</v>
@@ -1044,13 +1482,16 @@
       <c r="H36" t="n">
         <v>1.0</v>
       </c>
+      <c r="I36" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
-        <v>0.0</v>
+      <c r="A37" t="s">
+        <v>44</v>
       </c>
       <c r="B37" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C37" t="n">
         <v>1.0</v>
@@ -1070,10 +1511,13 @@
       <c r="H37" t="n">
         <v>1.0</v>
       </c>
+      <c r="I37" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>0.0</v>
+      <c r="A38" t="s">
+        <v>45</v>
       </c>
       <c r="B38" t="n">
         <v>0.0</v>
@@ -1082,7 +1526,7 @@
         <v>0.0</v>
       </c>
       <c r="D38" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E38" t="n">
         <v>1.0</v>
@@ -1096,10 +1540,13 @@
       <c r="H38" t="n">
         <v>1.0</v>
       </c>
+      <c r="I38" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
-        <v>1.0</v>
+      <c r="A39" t="s">
+        <v>46</v>
       </c>
       <c r="B39" t="n">
         <v>1.0</v>
@@ -1114,21 +1561,24 @@
         <v>1.0</v>
       </c>
       <c r="F39" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G39" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H39" t="n">
         <v>1.0</v>
       </c>
+      <c r="I39" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
-        <v>0.0</v>
+      <c r="A40" t="s">
+        <v>47</v>
       </c>
       <c r="B40" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C40" t="n">
         <v>1.0</v>
@@ -1148,10 +1598,13 @@
       <c r="H40" t="n">
         <v>1.0</v>
       </c>
+      <c r="I40" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
-        <v>0.0</v>
+      <c r="A41" t="s">
+        <v>48</v>
       </c>
       <c r="B41" t="n">
         <v>0.0</v>
@@ -1160,10 +1613,10 @@
         <v>0.0</v>
       </c>
       <c r="D41" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E41" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F41" t="n">
         <v>0.0</v>
@@ -1174,13 +1627,16 @@
       <c r="H41" t="n">
         <v>0.0</v>
       </c>
+      <c r="I41" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
-        <v>1.0</v>
+      <c r="A42" t="s">
+        <v>49</v>
       </c>
       <c r="B42" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C42" t="n">
         <v>0.0</v>
@@ -1200,10 +1656,13 @@
       <c r="H42" t="n">
         <v>0.0</v>
       </c>
+      <c r="I42" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>1.0</v>
+      <c r="A43" t="s">
+        <v>50</v>
       </c>
       <c r="B43" t="n">
         <v>1.0</v>
@@ -1212,10 +1671,10 @@
         <v>1.0</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E43" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F43" t="n">
         <v>1.0</v>
@@ -1226,19 +1685,22 @@
       <c r="H43" t="n">
         <v>1.0</v>
       </c>
+      <c r="I43" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
-        <v>0.0</v>
+      <c r="A44" t="s">
+        <v>51</v>
       </c>
       <c r="B44" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C44" t="n">
         <v>1.0</v>
       </c>
       <c r="D44" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E44" t="n">
         <v>0.0</v>
@@ -1252,13 +1714,16 @@
       <c r="H44" t="n">
         <v>0.0</v>
       </c>
+      <c r="I44" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>0.0</v>
+      <c r="A45" t="s">
+        <v>52</v>
       </c>
       <c r="B45" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C45" t="n">
         <v>1.0</v>
@@ -1278,10 +1743,13 @@
       <c r="H45" t="n">
         <v>1.0</v>
       </c>
+      <c r="I45" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
-        <v>1.0</v>
+      <c r="A46" t="s">
+        <v>53</v>
       </c>
       <c r="B46" t="n">
         <v>1.0</v>
@@ -1296,21 +1764,24 @@
         <v>1.0</v>
       </c>
       <c r="F46" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G46" t="n">
         <v>0.0</v>
       </c>
       <c r="H46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I46" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
-        <v>0.0</v>
+      <c r="A47" t="s">
+        <v>54</v>
       </c>
       <c r="B47" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C47" t="n">
         <v>1.0</v>
@@ -1330,10 +1801,13 @@
       <c r="H47" t="n">
         <v>1.0</v>
       </c>
+      <c r="I47" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
-        <v>1.0</v>
+      <c r="A48" t="s">
+        <v>55</v>
       </c>
       <c r="B48" t="n">
         <v>1.0</v>
@@ -1348,18 +1822,21 @@
         <v>1.0</v>
       </c>
       <c r="F48" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G48" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H48" t="n">
         <v>1.0</v>
       </c>
+      <c r="I48" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
-        <v>1.0</v>
+      <c r="A49" t="s">
+        <v>56</v>
       </c>
       <c r="B49" t="n">
         <v>1.0</v>
@@ -1374,18 +1851,21 @@
         <v>1.0</v>
       </c>
       <c r="F49" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G49" t="n">
         <v>0.0</v>
       </c>
       <c r="H49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I49" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
-        <v>1.0</v>
+      <c r="A50" t="s">
+        <v>57</v>
       </c>
       <c r="B50" t="n">
         <v>1.0</v>
@@ -1394,7 +1874,7 @@
         <v>1.0</v>
       </c>
       <c r="D50" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E50" t="n">
         <v>0.0</v>
@@ -1406,12 +1886,15 @@
         <v>0.0</v>
       </c>
       <c r="H50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I50" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
-        <v>1.0</v>
+      <c r="A51" t="s">
+        <v>58</v>
       </c>
       <c r="B51" t="n">
         <v>1.0</v>
@@ -1426,21 +1909,24 @@
         <v>1.0</v>
       </c>
       <c r="F51" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G51" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H51" t="n">
         <v>1.0</v>
       </c>
+      <c r="I51" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" t="n">
-        <v>0.0</v>
+      <c r="A52" t="s">
+        <v>59</v>
       </c>
       <c r="B52" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C52" t="n">
         <v>1.0</v>
@@ -1449,21 +1935,24 @@
         <v>1.0</v>
       </c>
       <c r="E52" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F52" t="n">
         <v>0.0</v>
       </c>
       <c r="G52" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H52" t="n">
         <v>1.0</v>
       </c>
+      <c r="I52" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="53">
-      <c r="A53" t="n">
-        <v>1.0</v>
+      <c r="A53" t="s">
+        <v>60</v>
       </c>
       <c r="B53" t="n">
         <v>1.0</v>
@@ -1478,21 +1967,24 @@
         <v>1.0</v>
       </c>
       <c r="F53" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G53" t="n">
         <v>0.0</v>
       </c>
       <c r="H53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I53" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="n">
-        <v>0.0</v>
+      <c r="A54" t="s">
+        <v>61</v>
       </c>
       <c r="B54" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C54" t="n">
         <v>1.0</v>
@@ -1512,13 +2004,16 @@
       <c r="H54" t="n">
         <v>1.0</v>
       </c>
+      <c r="I54" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" t="n">
-        <v>0.0</v>
+      <c r="A55" t="s">
+        <v>62</v>
       </c>
       <c r="B55" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C55" t="n">
         <v>1.0</v>
@@ -1538,10 +2033,13 @@
       <c r="H55" t="n">
         <v>1.0</v>
       </c>
+      <c r="I55" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" t="n">
-        <v>1.0</v>
+      <c r="A56" t="s">
+        <v>63</v>
       </c>
       <c r="B56" t="n">
         <v>1.0</v>
@@ -1556,18 +2054,21 @@
         <v>1.0</v>
       </c>
       <c r="F56" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G56" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H56" t="n">
         <v>1.0</v>
       </c>
+      <c r="I56" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="57">
-      <c r="A57" t="n">
-        <v>0.0</v>
+      <c r="A57" t="s">
+        <v>64</v>
       </c>
       <c r="B57" t="n">
         <v>0.0</v>
@@ -1582,21 +2083,24 @@
         <v>0.0</v>
       </c>
       <c r="F57" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G57" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H57" t="n">
         <v>0.0</v>
       </c>
+      <c r="I57" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" t="n">
-        <v>0.0</v>
+      <c r="A58" t="s">
+        <v>65</v>
       </c>
       <c r="B58" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C58" t="n">
         <v>1.0</v>
@@ -1616,10 +2120,13 @@
       <c r="H58" t="n">
         <v>1.0</v>
       </c>
+      <c r="I58" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" t="n">
-        <v>1.0</v>
+      <c r="A59" t="s">
+        <v>66</v>
       </c>
       <c r="B59" t="n">
         <v>1.0</v>
@@ -1628,7 +2135,7 @@
         <v>1.0</v>
       </c>
       <c r="D59" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E59" t="n">
         <v>0.0</v>
@@ -1642,10 +2149,13 @@
       <c r="H59" t="n">
         <v>0.0</v>
       </c>
+      <c r="I59" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" t="n">
-        <v>1.0</v>
+      <c r="A60" t="s">
+        <v>67</v>
       </c>
       <c r="B60" t="n">
         <v>1.0</v>
@@ -1660,18 +2170,21 @@
         <v>1.0</v>
       </c>
       <c r="F60" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G60" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H60" t="n">
         <v>1.0</v>
       </c>
+      <c r="I60" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="61">
-      <c r="A61" t="n">
-        <v>1.0</v>
+      <c r="A61" t="s">
+        <v>68</v>
       </c>
       <c r="B61" t="n">
         <v>1.0</v>
@@ -1680,7 +2193,7 @@
         <v>1.0</v>
       </c>
       <c r="D61" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E61" t="n">
         <v>0.0</v>
@@ -1692,15 +2205,18 @@
         <v>0.0</v>
       </c>
       <c r="H61" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I61" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="n">
-        <v>0.0</v>
+      <c r="A62" t="s">
+        <v>69</v>
       </c>
       <c r="B62" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C62" t="n">
         <v>1.0</v>
@@ -1709,10 +2225,10 @@
         <v>1.0</v>
       </c>
       <c r="E62" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F62" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G62" t="n">
         <v>1.0</v>
@@ -1720,10 +2236,13 @@
       <c r="H62" t="n">
         <v>1.0</v>
       </c>
+      <c r="I62" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" t="n">
-        <v>1.0</v>
+      <c r="A63" t="s">
+        <v>70</v>
       </c>
       <c r="B63" t="n">
         <v>1.0</v>
@@ -1738,18 +2257,21 @@
         <v>1.0</v>
       </c>
       <c r="F63" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G63" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H63" t="n">
         <v>1.0</v>
       </c>
+      <c r="I63" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" t="n">
-        <v>1.0</v>
+      <c r="A64" t="s">
+        <v>71</v>
       </c>
       <c r="B64" t="n">
         <v>1.0</v>
@@ -1764,18 +2286,21 @@
         <v>1.0</v>
       </c>
       <c r="F64" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G64" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H64" t="n">
         <v>1.0</v>
       </c>
+      <c r="I64" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="65">
-      <c r="A65" t="n">
-        <v>1.0</v>
+      <c r="A65" t="s">
+        <v>72</v>
       </c>
       <c r="B65" t="n">
         <v>1.0</v>
@@ -1790,18 +2315,21 @@
         <v>1.0</v>
       </c>
       <c r="F65" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G65" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H65" t="n">
         <v>1.0</v>
       </c>
+      <c r="I65" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="66">
-      <c r="A66" t="n">
-        <v>0.0</v>
+      <c r="A66" t="s">
+        <v>73</v>
       </c>
       <c r="B66" t="n">
         <v>0.0</v>
@@ -1822,12 +2350,15 @@
         <v>0.0</v>
       </c>
       <c r="H66" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I66" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="n">
-        <v>1.0</v>
+      <c r="A67" t="s">
+        <v>74</v>
       </c>
       <c r="B67" t="n">
         <v>1.0</v>
@@ -1842,21 +2373,24 @@
         <v>1.0</v>
       </c>
       <c r="F67" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G67" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H67" t="n">
         <v>1.0</v>
       </c>
+      <c r="I67" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="68">
-      <c r="A68" t="n">
-        <v>0.0</v>
+      <c r="A68" t="s">
+        <v>75</v>
       </c>
       <c r="B68" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C68" t="n">
         <v>1.0</v>
@@ -1865,7 +2399,7 @@
         <v>1.0</v>
       </c>
       <c r="E68" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F68" t="n">
         <v>0.0</v>
@@ -1876,10 +2410,13 @@
       <c r="H68" t="n">
         <v>0.0</v>
       </c>
+      <c r="I68" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="69">
-      <c r="A69" t="n">
-        <v>0.0</v>
+      <c r="A69" t="s">
+        <v>76</v>
       </c>
       <c r="B69" t="n">
         <v>0.0</v>
@@ -1888,7 +2425,7 @@
         <v>0.0</v>
       </c>
       <c r="D69" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E69" t="n">
         <v>1.0</v>
@@ -1902,10 +2439,13 @@
       <c r="H69" t="n">
         <v>1.0</v>
       </c>
+      <c r="I69" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="70">
-      <c r="A70" t="n">
-        <v>0.0</v>
+      <c r="A70" t="s">
+        <v>77</v>
       </c>
       <c r="B70" t="n">
         <v>0.0</v>
@@ -1917,10 +2457,10 @@
         <v>0.0</v>
       </c>
       <c r="E70" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F70" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G70" t="n">
         <v>0.0</v>
@@ -1928,10 +2468,13 @@
       <c r="H70" t="n">
         <v>0.0</v>
       </c>
+      <c r="I70" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="71">
-      <c r="A71" t="n">
-        <v>1.0</v>
+      <c r="A71" t="s">
+        <v>78</v>
       </c>
       <c r="B71" t="n">
         <v>1.0</v>
@@ -1946,18 +2489,21 @@
         <v>1.0</v>
       </c>
       <c r="F71" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G71" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H71" t="n">
         <v>1.0</v>
       </c>
+      <c r="I71" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="72">
-      <c r="A72" t="n">
-        <v>1.0</v>
+      <c r="A72" t="s">
+        <v>79</v>
       </c>
       <c r="B72" t="n">
         <v>1.0</v>
@@ -1972,18 +2518,21 @@
         <v>1.0</v>
       </c>
       <c r="F72" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G72" t="n">
         <v>0.0</v>
       </c>
       <c r="H72" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I72" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="n">
-        <v>1.0</v>
+      <c r="A73" t="s">
+        <v>80</v>
       </c>
       <c r="B73" t="n">
         <v>1.0</v>
@@ -1995,7 +2544,7 @@
         <v>1.0</v>
       </c>
       <c r="E73" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F73" t="n">
         <v>0.0</v>
@@ -2004,12 +2553,15 @@
         <v>0.0</v>
       </c>
       <c r="H73" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I73" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="n">
-        <v>1.0</v>
+      <c r="A74" t="s">
+        <v>81</v>
       </c>
       <c r="B74" t="n">
         <v>1.0</v>
@@ -2024,18 +2576,21 @@
         <v>1.0</v>
       </c>
       <c r="F74" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G74" t="n">
         <v>0.0</v>
       </c>
       <c r="H74" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I74" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="n">
-        <v>1.0</v>
+      <c r="A75" t="s">
+        <v>82</v>
       </c>
       <c r="B75" t="n">
         <v>1.0</v>
@@ -2047,7 +2602,7 @@
         <v>1.0</v>
       </c>
       <c r="E75" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F75" t="n">
         <v>0.0</v>
@@ -2058,10 +2613,13 @@
       <c r="H75" t="n">
         <v>0.0</v>
       </c>
+      <c r="I75" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="76">
-      <c r="A76" t="n">
-        <v>1.0</v>
+      <c r="A76" t="s">
+        <v>83</v>
       </c>
       <c r="B76" t="n">
         <v>1.0</v>
@@ -2070,7 +2628,7 @@
         <v>1.0</v>
       </c>
       <c r="D76" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E76" t="n">
         <v>0.0</v>
@@ -2084,10 +2642,13 @@
       <c r="H76" t="n">
         <v>0.0</v>
       </c>
+      <c r="I76" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="77">
-      <c r="A77" t="n">
-        <v>1.0</v>
+      <c r="A77" t="s">
+        <v>84</v>
       </c>
       <c r="B77" t="n">
         <v>1.0</v>
@@ -2096,7 +2657,7 @@
         <v>1.0</v>
       </c>
       <c r="D77" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E77" t="n">
         <v>0.0</v>
@@ -2110,10 +2671,13 @@
       <c r="H77" t="n">
         <v>0.0</v>
       </c>
+      <c r="I77" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="78">
-      <c r="A78" t="n">
-        <v>1.0</v>
+      <c r="A78" t="s">
+        <v>85</v>
       </c>
       <c r="B78" t="n">
         <v>1.0</v>
@@ -2128,18 +2692,21 @@
         <v>1.0</v>
       </c>
       <c r="F78" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G78" t="n">
         <v>0.0</v>
       </c>
       <c r="H78" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I78" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="n">
-        <v>1.0</v>
+      <c r="A79" t="s">
+        <v>86</v>
       </c>
       <c r="B79" t="n">
         <v>1.0</v>
@@ -2148,7 +2715,7 @@
         <v>1.0</v>
       </c>
       <c r="D79" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E79" t="n">
         <v>0.0</v>
@@ -2162,13 +2729,16 @@
       <c r="H79" t="n">
         <v>0.0</v>
       </c>
+      <c r="I79" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="80">
-      <c r="A80" t="n">
-        <v>0.0</v>
+      <c r="A80" t="s">
+        <v>87</v>
       </c>
       <c r="B80" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C80" t="n">
         <v>1.0</v>
@@ -2188,10 +2758,13 @@
       <c r="H80" t="n">
         <v>1.0</v>
       </c>
+      <c r="I80" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="81">
-      <c r="A81" t="n">
-        <v>1.0</v>
+      <c r="A81" t="s">
+        <v>88</v>
       </c>
       <c r="B81" t="n">
         <v>1.0</v>
@@ -2200,7 +2773,7 @@
         <v>1.0</v>
       </c>
       <c r="D81" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E81" t="n">
         <v>0.0</v>
@@ -2214,10 +2787,13 @@
       <c r="H81" t="n">
         <v>0.0</v>
       </c>
+      <c r="I81" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="82">
-      <c r="A82" t="n">
-        <v>1.0</v>
+      <c r="A82" t="s">
+        <v>89</v>
       </c>
       <c r="B82" t="n">
         <v>1.0</v>
@@ -2226,7 +2802,7 @@
         <v>1.0</v>
       </c>
       <c r="D82" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E82" t="n">
         <v>0.0</v>
@@ -2240,10 +2816,13 @@
       <c r="H82" t="n">
         <v>0.0</v>
       </c>
+      <c r="I82" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="83">
-      <c r="A83" t="n">
-        <v>1.0</v>
+      <c r="A83" t="s">
+        <v>90</v>
       </c>
       <c r="B83" t="n">
         <v>1.0</v>
@@ -2258,18 +2837,21 @@
         <v>1.0</v>
       </c>
       <c r="F83" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G83" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H83" t="n">
         <v>1.0</v>
       </c>
+      <c r="I83" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="84">
-      <c r="A84" t="n">
-        <v>1.0</v>
+      <c r="A84" t="s">
+        <v>91</v>
       </c>
       <c r="B84" t="n">
         <v>1.0</v>
@@ -2284,27 +2866,30 @@
         <v>1.0</v>
       </c>
       <c r="F84" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G84" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H84" t="n">
         <v>1.0</v>
       </c>
+      <c r="I84" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="85">
-      <c r="A85" t="n">
-        <v>0.0</v>
+      <c r="A85" t="s">
+        <v>92</v>
       </c>
       <c r="B85" t="n">
         <v>0.0</v>
       </c>
       <c r="C85" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D85" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E85" t="n">
         <v>0.0</v>
@@ -2316,6 +2901,9 @@
         <v>0.0</v>
       </c>
       <c r="H85" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I85" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2334,30 +2922,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>96</v>
+      </c>
+      <c r="F1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>0.0</v>
+      <c r="A2" t="s">
+        <v>98</v>
       </c>
       <c r="B2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D2" t="n">
         <v>0.0</v>
@@ -2365,13 +2956,16 @@
       <c r="E2" t="n">
         <v>0.0</v>
       </c>
+      <c r="F2" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1.0</v>
+      <c r="A3" t="s">
+        <v>99</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
@@ -2382,13 +2976,16 @@
       <c r="E3" t="n">
         <v>0.0</v>
       </c>
+      <c r="F3" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>0.0</v>
+      <c r="A4" t="s">
+        <v>100</v>
       </c>
       <c r="B4" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
@@ -2397,15 +2994,18 @@
         <v>1.0</v>
       </c>
       <c r="E4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F4" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>0.0</v>
+      <c r="A5" t="s">
+        <v>101</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C5" t="n">
         <v>1.0</v>
@@ -2414,15 +3014,18 @@
         <v>1.0</v>
       </c>
       <c r="E5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F5" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>0.0</v>
+      <c r="A6" t="s">
+        <v>102</v>
       </c>
       <c r="B6" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C6" t="n">
         <v>1.0</v>
@@ -2431,15 +3034,18 @@
         <v>1.0</v>
       </c>
       <c r="E6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F6" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>0.0</v>
+      <c r="A7" t="s">
+        <v>103</v>
       </c>
       <c r="B7" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C7" t="n">
         <v>1.0</v>
@@ -2448,32 +3054,38 @@
         <v>1.0</v>
       </c>
       <c r="E7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F7" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>0.0</v>
+      <c r="A8" t="s">
+        <v>104</v>
       </c>
       <c r="B8" t="n">
         <v>0.0</v>
       </c>
       <c r="C8" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D8" t="n">
         <v>1.0</v>
       </c>
       <c r="E8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F8" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>1.0</v>
+      <c r="A9" t="s">
+        <v>105</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C9" t="n">
         <v>0.0</v>
@@ -2484,13 +3096,16 @@
       <c r="E9" t="n">
         <v>0.0</v>
       </c>
+      <c r="F9" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>1.0</v>
+      <c r="A10" t="s">
+        <v>106</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C10" t="n">
         <v>0.0</v>
@@ -2501,13 +3116,16 @@
       <c r="E10" t="n">
         <v>0.0</v>
       </c>
+      <c r="F10" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>1.0</v>
+      <c r="A11" t="s">
+        <v>107</v>
       </c>
       <c r="B11" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C11" t="n">
         <v>0.0</v>
@@ -2518,16 +3136,19 @@
       <c r="E11" t="n">
         <v>0.0</v>
       </c>
+      <c r="F11" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>0.0</v>
+      <c r="A12" t="s">
+        <v>108</v>
       </c>
       <c r="B12" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D12" t="n">
         <v>0.0</v>
@@ -2535,16 +3156,19 @@
       <c r="E12" t="n">
         <v>0.0</v>
       </c>
+      <c r="F12" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>0.0</v>
+      <c r="A13" t="s">
+        <v>109</v>
       </c>
       <c r="B13" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D13" t="n">
         <v>0.0</v>
@@ -2552,33 +3176,39 @@
       <c r="E13" t="n">
         <v>0.0</v>
       </c>
+      <c r="F13" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>1.0</v>
+      <c r="A14" t="s">
+        <v>110</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C14" t="n">
         <v>0.0</v>
       </c>
       <c r="D14" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F14" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>0.0</v>
+      <c r="A15" t="s">
+        <v>111</v>
       </c>
       <c r="B15" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D15" t="n">
         <v>0.0</v>
@@ -2586,16 +3216,19 @@
       <c r="E15" t="n">
         <v>0.0</v>
       </c>
+      <c r="F15" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>0.0</v>
+      <c r="A16" t="s">
+        <v>112</v>
       </c>
       <c r="B16" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D16" t="n">
         <v>0.0</v>
@@ -2603,10 +3236,13 @@
       <c r="E16" t="n">
         <v>0.0</v>
       </c>
+      <c r="F16" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>0.0</v>
+      <c r="A17" t="s">
+        <v>113</v>
       </c>
       <c r="B17" t="n">
         <v>0.0</v>
@@ -2615,15 +3251,18 @@
         <v>0.0</v>
       </c>
       <c r="D17" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F17" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>0.0</v>
+      <c r="A18" t="s">
+        <v>114</v>
       </c>
       <c r="B18" t="n">
         <v>0.0</v>
@@ -2632,35 +3271,41 @@
         <v>0.0</v>
       </c>
       <c r="D18" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F18" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>0.0</v>
+      <c r="A19" t="s">
+        <v>115</v>
       </c>
       <c r="B19" t="n">
         <v>0.0</v>
       </c>
       <c r="C19" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E19" t="n">
         <v>0.0</v>
       </c>
+      <c r="F19" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>1.0</v>
+      <c r="A20" t="s">
+        <v>116</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C20" t="n">
         <v>0.0</v>
@@ -2671,16 +3316,19 @@
       <c r="E20" t="n">
         <v>0.0</v>
       </c>
+      <c r="F20" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>0.0</v>
+      <c r="A21" t="s">
+        <v>117</v>
       </c>
       <c r="B21" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D21" t="n">
         <v>0.0</v>
@@ -2688,10 +3336,13 @@
       <c r="E21" t="n">
         <v>0.0</v>
       </c>
+      <c r="F21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>0.0</v>
+      <c r="A22" t="s">
+        <v>118</v>
       </c>
       <c r="B22" t="n">
         <v>0.0</v>
@@ -2700,15 +3351,18 @@
         <v>0.0</v>
       </c>
       <c r="D22" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F22" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>0.0</v>
+      <c r="A23" t="s">
+        <v>119</v>
       </c>
       <c r="B23" t="n">
         <v>0.0</v>
@@ -2717,15 +3371,18 @@
         <v>0.0</v>
       </c>
       <c r="D23" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F23" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>0.0</v>
+      <c r="A24" t="s">
+        <v>120</v>
       </c>
       <c r="B24" t="n">
         <v>0.0</v>
@@ -2734,18 +3391,21 @@
         <v>0.0</v>
       </c>
       <c r="D24" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E24" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F24" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>0.0</v>
+      <c r="A25" t="s">
+        <v>121</v>
       </c>
       <c r="B25" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C25" t="n">
         <v>1.0</v>
@@ -2754,6 +3414,9 @@
         <v>1.0</v>
       </c>
       <c r="E25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2772,56 +3435,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>123</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1.0</v>
+      <c r="A2" t="s">
+        <v>106</v>
       </c>
       <c r="B2" t="n">
         <v>1.0</v>
       </c>
       <c r="C2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D2" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1.0</v>
+      <c r="A3" t="s">
+        <v>122</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
       </c>
+      <c r="D3" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>0.0</v>
+      <c r="A4" t="s">
+        <v>124</v>
       </c>
       <c r="B4" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D4" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>0.0</v>
+      <c r="A5" t="s">
+        <v>125</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D5" t="n">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>